<commit_message>
adding new output data test
</commit_message>
<xml_diff>
--- a/output/system_consideration.xlsx
+++ b/output/system_consideration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politecnicobari-my.sharepoint.com/personal/a_milella9_studenti_poliba_it/Documents/Personal-Surface/Carriera/Borsa COMAU/INIZIO LAVORI/03 GIUGNO/GIT/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="580" documentId="8_{26AC92F0-D54C-475B-82CA-E79DDC85AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{512DD2B2-C9D8-4DE9-AA9F-99CDDF4639FC}"/>
+  <xr:revisionPtr revIDLastSave="581" documentId="8_{26AC92F0-D54C-475B-82CA-E79DDC85AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29BADD7E-81D2-4E49-A248-E2B54943CE7F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="588" activeTab="6" xr2:uid="{7B77A073-3631-4C57-A8A1-A6F8804CA2BE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="236">
   <si>
     <t>image_name</t>
   </si>
@@ -21666,8 +21666,8 @@
   </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -22275,6 +22275,12 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="H30" s="8" t="s">
         <v>59</v>
       </c>
@@ -22283,6 +22289,12 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
       <c r="H31" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
adding pdf consideration file
</commit_message>
<xml_diff>
--- a/output/system_consideration.xlsx
+++ b/output/system_consideration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politecnicobari-my.sharepoint.com/personal/a_milella9_studenti_poliba_it/Documents/Personal-Surface/Carriera/Borsa COMAU/INIZIO LAVORI/03 GIUGNO/GIT/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="581" documentId="8_{26AC92F0-D54C-475B-82CA-E79DDC85AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29BADD7E-81D2-4E49-A248-E2B54943CE7F}"/>
+  <xr:revisionPtr revIDLastSave="585" documentId="8_{26AC92F0-D54C-475B-82CA-E79DDC85AD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB4BFAE7-4A20-4CBA-AED1-C984C59A412D}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="588" activeTab="6" xr2:uid="{7B77A073-3631-4C57-A8A1-A6F8804CA2BE}"/>
   </bookViews>
@@ -735,19 +735,20 @@
     <t>Dev St</t>
   </si>
   <si>
-    <t>185 row</t>
-  </si>
-  <si>
     <t>38 row</t>
   </si>
   <si>
     <t>100 row</t>
   </si>
   <si>
-    <t>47 row</t>
-  </si>
-  <si>
     <t>46 row</t>
+  </si>
+  <si>
+    <t>HALCON elapsed
+time ms</t>
+  </si>
+  <si>
+    <t>184 row</t>
   </si>
 </sst>
 </file>
@@ -1280,19 +1281,19 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1677,8 +1678,8 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6327,8 +6328,8 @@
   </sheetPr>
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView topLeftCell="I1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8416,7 +8417,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16295,8 +16296,8 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView topLeftCell="H77" zoomScale="101" workbookViewId="0">
-      <selection activeCell="L77" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="H1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21667,7 +21668,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21684,26 +21685,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
-        <v>232</v>
+      <c r="I1" s="10"/>
+      <c r="J1" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
@@ -21865,26 +21866,26 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7" t="s">
-        <v>233</v>
+      <c r="I9" s="10"/>
+      <c r="J9" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -22041,26 +22042,26 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7" t="s">
-        <v>235</v>
+      <c r="I17" s="10"/>
+      <c r="J17" s="6" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
@@ -22228,12 +22229,12 @@
       <c r="B25" s="9"/>
       <c r="C25"/>
       <c r="H25" s="9" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="8" t="s">
         <v>229</v>
       </c>
       <c r="B26">
@@ -22241,7 +22242,7 @@
         <v>115.84594594594597</v>
       </c>
       <c r="C26"/>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="8" t="s">
         <v>229</v>
       </c>
       <c r="I26">
@@ -22250,7 +22251,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="8" t="s">
         <v>230</v>
       </c>
       <c r="B27">
@@ -22258,7 +22259,7 @@
         <v>58.47814527943877</v>
       </c>
       <c r="C27"/>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="8" t="s">
         <v>230</v>
       </c>
       <c r="I27">
@@ -22267,24 +22268,24 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>231</v>
+      <c r="A28" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>